<commit_message>
Update tests/ and tutorials/
</commit_message>
<xml_diff>
--- a/tutorials/excel_template.xlsx
+++ b/tutorials/excel_template.xlsx
@@ -18,7 +18,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="26">
+  <si>
+    <t>PENDRAGON</t>
+  </si>
+  <si>
+    <t>LE GAULOIS</t>
+  </si>
+  <si>
+    <t>DE VANNES</t>
+  </si>
+  <si>
+    <t>DU LAC</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>Provençal</t>
+  </si>
+  <si>
+    <t>Karadoc</t>
+  </si>
+  <si>
+    <t>Lancelot</t>
+  </si>
   <si>
     <t>Numéro</t>
   </si>
@@ -50,7 +74,7 @@
     <t>Poursuivez vos efforts !</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>Ceci est une remarque</t>
   </si>
   <si>
     <t>Soin</t>
@@ -538,7 +562,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -549,23 +573,65 @@
   <sheetData>
     <row r="1" spans="1:4" ht="37.5" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="25" customHeight="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="25" customHeight="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="25" customHeight="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="25" customHeight="1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="25" customHeight="1">
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="25" customHeight="1">
-      <c r="D3" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
@@ -578,6 +644,16 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="expression" dxfId="0" priority="7">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="expression" dxfId="0" priority="10">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B2">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>Classe!D2</formula>
@@ -588,6 +664,16 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="expression" dxfId="0" priority="8">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="0" priority="11">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C2">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>Classe!D2</formula>
@@ -598,11 +684,27 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <conditionalFormatting sqref="C4">
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="expression" dxfId="0" priority="12">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
       <formula1>"True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>
@@ -612,7 +714,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -623,39 +725,36 @@
   <sheetData>
     <row r="1" spans="1:7" ht="37.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="25" customHeight="1">
       <c r="A2" s="1">
-        <f>Classe!A2</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <f>Classe!B2</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <f>Classe!C2</f>
-        <v>0</v>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D2" s="1">
         <v>-1</v>
@@ -673,16 +772,13 @@
     </row>
     <row r="3" spans="1:7" ht="25" customHeight="1">
       <c r="A3" s="1">
-        <f>Classe!A3</f>
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <f>Classe!B3</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <f>Classe!C3</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="D3" s="1">
         <v>-1</v>
@@ -698,6 +794,54 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:7" ht="25" customHeight="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="1">
+        <f>IF(AND(Classe!D4=FALSE(), D4&lt;&gt;-1, E4&lt;&gt;-1, F4&lt;&gt;-1),SUM(D4:F4),NA())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="25" customHeight="1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G5" s="1">
+        <f>IF(AND(Classe!D5=FALSE(), D5&lt;&gt;-1, E5&lt;&gt;-1, F5&lt;&gt;-1),SUM(D5:F5),NA())</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -709,6 +853,16 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="expression" dxfId="0" priority="15">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="expression" dxfId="0" priority="22">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B2">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>Classe!D2</formula>
@@ -719,6 +873,16 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="expression" dxfId="0" priority="16">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="0" priority="23">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C2">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>Classe!D2</formula>
@@ -729,23 +893,33 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="expression" dxfId="0" priority="17">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="expression" dxfId="0" priority="24">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D2">
     <cfRule type="expression" dxfId="0" priority="4">
       <formula>Classe!D2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="29" operator="between">
       <formula>0</formula>
       <formula>0.33</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="30" operator="between">
       <formula>0.33</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="31" operator="between">
       <formula>0.66</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="32" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -753,19 +927,59 @@
     <cfRule type="expression" dxfId="0" priority="11">
       <formula>Classe!D3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="27" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="41" operator="between">
       <formula>0</formula>
       <formula>0.33</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="42" operator="between">
       <formula>0.33</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="29" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="43" operator="between">
       <formula>0.66</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="30" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="44" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="expression" dxfId="0" priority="18">
+      <formula>Classe!D4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="53" operator="between">
+      <formula>0</formula>
+      <formula>0.33</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="54" operator="between">
+      <formula>0.33</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="55" operator="between">
+      <formula>0.66</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="56" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="expression" dxfId="0" priority="25">
+      <formula>Classe!D5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="65" operator="between">
+      <formula>0</formula>
+      <formula>0.33</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="66" operator="between">
+      <formula>0.33</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="67" operator="between">
+      <formula>0.66</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="68" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -773,19 +987,19 @@
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>Classe!D2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="19" operator="between">
-      <formula>0</formula>
-      <formula>0.66</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="33" operator="between">
+      <formula>0</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="34" operator="between">
       <formula>0.66</formula>
       <formula>1.32</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="21" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="35" operator="between">
       <formula>1.32</formula>
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="36" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -793,19 +1007,59 @@
     <cfRule type="expression" dxfId="0" priority="12">
       <formula>Classe!D3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="31" operator="between">
-      <formula>0</formula>
-      <formula>0.66</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="32" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="45" operator="between">
+      <formula>0</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="46" operator="between">
       <formula>0.66</formula>
       <formula>1.32</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="33" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="47" operator="between">
       <formula>1.32</formula>
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="48" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="expression" dxfId="0" priority="19">
+      <formula>Classe!D4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="57" operator="between">
+      <formula>0</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="58" operator="between">
+      <formula>0.66</formula>
+      <formula>1.32</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="59" operator="between">
+      <formula>1.32</formula>
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="60" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="expression" dxfId="0" priority="26">
+      <formula>Classe!D5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="69" operator="between">
+      <formula>0</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="70" operator="between">
+      <formula>0.66</formula>
+      <formula>1.32</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="71" operator="between">
+      <formula>1.32</formula>
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="72" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -813,19 +1067,19 @@
     <cfRule type="expression" dxfId="0" priority="6">
       <formula>Classe!D2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="23" operator="between">
-      <formula>0</formula>
-      <formula>0.66</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="37" operator="between">
+      <formula>0</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="38" operator="between">
       <formula>0.66</formula>
       <formula>1.32</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="39" operator="between">
       <formula>1.32</formula>
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="40" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -833,19 +1087,59 @@
     <cfRule type="expression" dxfId="0" priority="13">
       <formula>Classe!D3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="35" operator="between">
-      <formula>0</formula>
-      <formula>0.66</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="36" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="49" operator="between">
+      <formula>0</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="50" operator="between">
       <formula>0.66</formula>
       <formula>1.32</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="37" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="51" operator="between">
       <formula>1.32</formula>
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="38" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="52" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4">
+    <cfRule type="expression" dxfId="0" priority="20">
+      <formula>Classe!D4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="61" operator="between">
+      <formula>0</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="62" operator="between">
+      <formula>0.66</formula>
+      <formula>1.32</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="63" operator="between">
+      <formula>1.32</formula>
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="64" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="expression" dxfId="0" priority="27">
+      <formula>Classe!D5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="73" operator="between">
+      <formula>0</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="74" operator="between">
+      <formula>0.66</formula>
+      <formula>1.32</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="75" operator="between">
+      <formula>1.32</formula>
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="76" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -859,7 +1153,17 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="6">
+  <conditionalFormatting sqref="G4">
+    <cfRule type="expression" dxfId="0" priority="21">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="expression" dxfId="0" priority="28">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="input" sqref="D2">
       <formula1>"0,1"</formula1>
     </dataValidation>
@@ -876,6 +1180,24 @@
       <formula1>"0,1,2"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="input" sqref="F3">
+      <formula1>"0,0.5,1,1.5,2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="input" sqref="D4">
+      <formula1>"0,1"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="input" sqref="E4">
+      <formula1>"0,1,2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="input" sqref="F4">
+      <formula1>"0,0.5,1,1.5,2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="input" sqref="D5">
+      <formula1>"0,1"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="input" sqref="E5">
+      <formula1>"0,1,2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="input" sqref="F5">
       <formula1>"0,0.5,1,1.5,2"</formula1>
     </dataValidation>
   </dataValidations>
@@ -885,7 +1207,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -896,36 +1218,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="37.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="25" customHeight="1">
       <c r="A2" s="1">
-        <f>Classe!A2</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <f>Classe!B2</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <f>Classe!C2</f>
-        <v>0</v>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E2" s="3" t="str">
         <f>IF(SUM(Notes!E2)/2&lt;0.5,TRUE,FALSE)</f>
@@ -935,16 +1254,13 @@
     </row>
     <row r="3" spans="1:6" ht="25" customHeight="1">
       <c r="A3" s="1">
-        <f>Classe!A3</f>
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <f>Classe!B3</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <f>Classe!C3</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="E3" s="3" t="str">
         <f>IF(SUM(Notes!E3)/2&lt;0.5,TRUE,FALSE)</f>
@@ -952,6 +1268,38 @@
       </c>
       <c r="F3" s="1"/>
     </row>
+    <row r="4" spans="1:6" ht="25" customHeight="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="str">
+        <f>IF(SUM(Notes!E4)/2&lt;0.5,TRUE,FALSE)</f>
+        <v>autofill</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="25" customHeight="1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="str">
+        <f>IF(SUM(Notes!E5)/2&lt;0.5,TRUE,FALSE)</f>
+        <v>autofill</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -963,6 +1311,16 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="expression" dxfId="0" priority="13">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="expression" dxfId="0" priority="19">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B2">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>Classe!D2</formula>
@@ -973,6 +1331,16 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="expression" dxfId="0" priority="14">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="0" priority="20">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C2">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>Classe!D2</formula>
@@ -983,6 +1351,16 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="expression" dxfId="0" priority="15">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="expression" dxfId="0" priority="21">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D2">
     <cfRule type="expression" dxfId="0" priority="4">
       <formula>Classe!D2</formula>
@@ -993,6 +1371,16 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="expression" dxfId="0" priority="16">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="expression" dxfId="0" priority="22">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E2">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>Classe!D2</formula>
@@ -1003,6 +1391,16 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="expression" dxfId="0" priority="17">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="expression" dxfId="0" priority="23">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F2">
     <cfRule type="expression" dxfId="0" priority="6">
       <formula>Classe!D2</formula>
@@ -1013,11 +1411,27 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <conditionalFormatting sqref="F4">
+    <cfRule type="expression" dxfId="0" priority="18">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="expression" dxfId="0" priority="24">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
       <formula1>"True,False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1027,7 +1441,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1038,60 +1452,86 @@
   <sheetData>
     <row r="1" spans="1:6" ht="37.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="25" customHeight="1">
       <c r="A2" s="1">
-        <f>Classe!A2</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <f>Classe!B2</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <f>Classe!C2</f>
-        <v>0</v>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25" customHeight="1">
       <c r="A3" s="1">
-        <f>Classe!A3</f>
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <f>Classe!B3</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <f>Classe!C3</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="25" customHeight="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25" customHeight="1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1105,6 +1545,16 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="expression" dxfId="0" priority="13">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="expression" dxfId="0" priority="19">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B2">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>Classe!D2</formula>
@@ -1115,6 +1565,16 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="expression" dxfId="0" priority="14">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="0" priority="20">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C2">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>Classe!D2</formula>
@@ -1125,17 +1585,27 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="expression" dxfId="0" priority="15">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="expression" dxfId="0" priority="21">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D2">
     <cfRule type="expression" dxfId="0" priority="4">
       <formula>Classe!D2</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="13" operator="containsText" text="Non acquis">
+    <cfRule type="containsText" dxfId="1" priority="25" operator="containsText" text="Non acquis">
       <formula>NOT(ISERROR(SEARCH("Non acquis",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="14" operator="containsText" text="En voie d'acquisition">
+    <cfRule type="containsText" dxfId="2" priority="26" operator="containsText" text="En voie d'acquisition">
       <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="Acquis">
+    <cfRule type="containsText" dxfId="3" priority="27" operator="containsText" text="Acquis">
       <formula>NOT(ISERROR(SEARCH("Acquis",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1143,27 +1613,55 @@
     <cfRule type="expression" dxfId="0" priority="10">
       <formula>Classe!D3</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="22" operator="containsText" text="Non acquis">
+    <cfRule type="containsText" dxfId="1" priority="34" operator="containsText" text="Non acquis">
       <formula>NOT(ISERROR(SEARCH("Non acquis",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="23" operator="containsText" text="En voie d'acquisition">
+    <cfRule type="containsText" dxfId="2" priority="35" operator="containsText" text="En voie d'acquisition">
       <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="24" operator="containsText" text="Acquis">
+    <cfRule type="containsText" dxfId="3" priority="36" operator="containsText" text="Acquis">
       <formula>NOT(ISERROR(SEARCH("Acquis",D3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="expression" dxfId="0" priority="16">
+      <formula>Classe!D4</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="43" operator="containsText" text="Non acquis">
+      <formula>NOT(ISERROR(SEARCH("Non acquis",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="44" operator="containsText" text="En voie d'acquisition">
+      <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="45" operator="containsText" text="Acquis">
+      <formula>NOT(ISERROR(SEARCH("Acquis",D4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="expression" dxfId="0" priority="22">
+      <formula>Classe!D5</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="52" operator="containsText" text="Non acquis">
+      <formula>NOT(ISERROR(SEARCH("Non acquis",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="53" operator="containsText" text="En voie d'acquisition">
+      <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="54" operator="containsText" text="Acquis">
+      <formula>NOT(ISERROR(SEARCH("Acquis",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>Classe!D2</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="16" operator="containsText" text="Non acquis">
+    <cfRule type="containsText" dxfId="1" priority="28" operator="containsText" text="Non acquis">
       <formula>NOT(ISERROR(SEARCH("Non acquis",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="17" operator="containsText" text="En voie d'acquisition">
+    <cfRule type="containsText" dxfId="2" priority="29" operator="containsText" text="En voie d'acquisition">
       <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="18" operator="containsText" text="Acquis">
+    <cfRule type="containsText" dxfId="3" priority="30" operator="containsText" text="Acquis">
       <formula>NOT(ISERROR(SEARCH("Acquis",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1171,27 +1669,55 @@
     <cfRule type="expression" dxfId="0" priority="11">
       <formula>Classe!D3</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="25" operator="containsText" text="Non acquis">
+    <cfRule type="containsText" dxfId="1" priority="37" operator="containsText" text="Non acquis">
       <formula>NOT(ISERROR(SEARCH("Non acquis",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="26" operator="containsText" text="En voie d'acquisition">
+    <cfRule type="containsText" dxfId="2" priority="38" operator="containsText" text="En voie d'acquisition">
       <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="27" operator="containsText" text="Acquis">
+    <cfRule type="containsText" dxfId="3" priority="39" operator="containsText" text="Acquis">
       <formula>NOT(ISERROR(SEARCH("Acquis",E3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="expression" dxfId="0" priority="17">
+      <formula>Classe!D4</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="46" operator="containsText" text="Non acquis">
+      <formula>NOT(ISERROR(SEARCH("Non acquis",E4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="47" operator="containsText" text="En voie d'acquisition">
+      <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",E4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="48" operator="containsText" text="Acquis">
+      <formula>NOT(ISERROR(SEARCH("Acquis",E4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="expression" dxfId="0" priority="23">
+      <formula>Classe!D5</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="55" operator="containsText" text="Non acquis">
+      <formula>NOT(ISERROR(SEARCH("Non acquis",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="56" operator="containsText" text="En voie d'acquisition">
+      <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="57" operator="containsText" text="Acquis">
+      <formula>NOT(ISERROR(SEARCH("Acquis",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
     <cfRule type="expression" dxfId="0" priority="6">
       <formula>Classe!D2</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="19" operator="containsText" text="Non acquis">
+    <cfRule type="containsText" dxfId="1" priority="31" operator="containsText" text="Non acquis">
       <formula>NOT(ISERROR(SEARCH("Non acquis",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="20" operator="containsText" text="En voie d'acquisition">
+    <cfRule type="containsText" dxfId="2" priority="32" operator="containsText" text="En voie d'acquisition">
       <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="21" operator="containsText" text="Acquis">
+    <cfRule type="containsText" dxfId="3" priority="33" operator="containsText" text="Acquis">
       <formula>NOT(ISERROR(SEARCH("Acquis",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1199,17 +1725,45 @@
     <cfRule type="expression" dxfId="0" priority="12">
       <formula>Classe!D3</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="28" operator="containsText" text="Non acquis">
+    <cfRule type="containsText" dxfId="1" priority="40" operator="containsText" text="Non acquis">
       <formula>NOT(ISERROR(SEARCH("Non acquis",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="29" operator="containsText" text="En voie d'acquisition">
+    <cfRule type="containsText" dxfId="2" priority="41" operator="containsText" text="En voie d'acquisition">
       <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="30" operator="containsText" text="Acquis">
+    <cfRule type="containsText" dxfId="3" priority="42" operator="containsText" text="Acquis">
       <formula>NOT(ISERROR(SEARCH("Acquis",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="6">
+  <conditionalFormatting sqref="F4">
+    <cfRule type="expression" dxfId="0" priority="18">
+      <formula>Classe!D4</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="49" operator="containsText" text="Non acquis">
+      <formula>NOT(ISERROR(SEARCH("Non acquis",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="50" operator="containsText" text="En voie d'acquisition">
+      <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="51" operator="containsText" text="Acquis">
+      <formula>NOT(ISERROR(SEARCH("Acquis",F4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="expression" dxfId="0" priority="24">
+      <formula>Classe!D5</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="58" operator="containsText" text="Non acquis">
+      <formula>NOT(ISERROR(SEARCH("Non acquis",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="59" operator="containsText" text="En voie d'acquisition">
+      <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="60" operator="containsText" text="Acquis">
+      <formula>NOT(ISERROR(SEARCH("Acquis",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
       <formula1>"Non acquis,En voie d'acquisition,Acquis"</formula1>
     </dataValidation>
@@ -1226,6 +1780,24 @@
       <formula1>"Non acquis,En voie d'acquisition,Acquis"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3">
+      <formula1>"Non acquis,En voie d'acquisition,Acquis"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4">
+      <formula1>"Non acquis,En voie d'acquisition,Acquis"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">
+      <formula1>"Non acquis,En voie d'acquisition,Acquis"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4">
+      <formula1>"Non acquis,En voie d'acquisition,Acquis"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5">
+      <formula1>"Non acquis,En voie d'acquisition,Acquis"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5">
+      <formula1>"Non acquis,En voie d'acquisition,Acquis"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5">
       <formula1>"Non acquis,En voie d'acquisition,Acquis"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1235,7 +1807,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1246,61 +1818,91 @@
   <sheetData>
     <row r="1" spans="1:5" ht="37.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="25" customHeight="1">
       <c r="A2" s="1">
-        <f>Classe!A2</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <f>Classe!B2</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <f>Classe!C2</f>
-        <v>0</v>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>IF(SUM(Notes!D2, Notes!E2)/3&lt;0.8, IF(SUM(Notes!D2, Notes!E2)/3&lt;0.4,"Non acquis","En voie d'acquisition"),"Acquis")</f>
         <v>autofill</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25" customHeight="1">
       <c r="A3" s="1">
-        <f>Classe!A3</f>
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <f>Classe!B3</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <f>Classe!C3</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="str">
         <f>IF(SUM(Notes!D3, Notes!E3)/3&lt;0.8, IF(SUM(Notes!D3, Notes!E3)/3&lt;0.4,"Non acquis","En voie d'acquisition"),"Acquis")</f>
         <v>autofill</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="25" customHeight="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f>IF(SUM(Notes!D4, Notes!E4)/3&lt;0.8, IF(SUM(Notes!D4, Notes!E4)/3&lt;0.4,"Non acquis","En voie d'acquisition"),"Acquis")</f>
+        <v>autofill</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="25" customHeight="1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>IF(SUM(Notes!D5, Notes!E5)/3&lt;0.8, IF(SUM(Notes!D5, Notes!E5)/3&lt;0.4,"Non acquis","En voie d'acquisition"),"Acquis")</f>
+        <v>autofill</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1314,6 +1916,16 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="expression" dxfId="0" priority="11">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="expression" dxfId="0" priority="16">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B2">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>Classe!D2</formula>
@@ -1324,6 +1936,16 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="expression" dxfId="0" priority="12">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="0" priority="17">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C2">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>Classe!D2</formula>
@@ -1334,17 +1956,27 @@
       <formula>Classe!D3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="expression" dxfId="0" priority="13">
+      <formula>Classe!D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="expression" dxfId="0" priority="18">
+      <formula>Classe!D5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D2">
     <cfRule type="expression" dxfId="0" priority="4">
       <formula>Classe!D2</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="Non acquis">
+    <cfRule type="containsText" dxfId="1" priority="21" operator="containsText" text="Non acquis">
       <formula>NOT(ISERROR(SEARCH("Non acquis",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="En voie d'acquisition">
+    <cfRule type="containsText" dxfId="2" priority="22" operator="containsText" text="En voie d'acquisition">
       <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="Acquis">
+    <cfRule type="containsText" dxfId="3" priority="23" operator="containsText" text="Acquis">
       <formula>NOT(ISERROR(SEARCH("Acquis",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1352,27 +1984,55 @@
     <cfRule type="expression" dxfId="0" priority="9">
       <formula>Classe!D3</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="17" operator="containsText" text="Non acquis">
+    <cfRule type="containsText" dxfId="1" priority="27" operator="containsText" text="Non acquis">
       <formula>NOT(ISERROR(SEARCH("Non acquis",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="18" operator="containsText" text="En voie d'acquisition">
+    <cfRule type="containsText" dxfId="2" priority="28" operator="containsText" text="En voie d'acquisition">
       <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="19" operator="containsText" text="Acquis">
+    <cfRule type="containsText" dxfId="3" priority="29" operator="containsText" text="Acquis">
       <formula>NOT(ISERROR(SEARCH("Acquis",D3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="expression" dxfId="0" priority="14">
+      <formula>Classe!D4</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="33" operator="containsText" text="Non acquis">
+      <formula>NOT(ISERROR(SEARCH("Non acquis",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="34" operator="containsText" text="En voie d'acquisition">
+      <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="35" operator="containsText" text="Acquis">
+      <formula>NOT(ISERROR(SEARCH("Acquis",D4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="expression" dxfId="0" priority="19">
+      <formula>Classe!D5</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="39" operator="containsText" text="Non acquis">
+      <formula>NOT(ISERROR(SEARCH("Non acquis",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="40" operator="containsText" text="En voie d'acquisition">
+      <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="41" operator="containsText" text="Acquis">
+      <formula>NOT(ISERROR(SEARCH("Acquis",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>Classe!D2</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="14" operator="containsText" text="Non acquis">
+    <cfRule type="containsText" dxfId="1" priority="24" operator="containsText" text="Non acquis">
       <formula>NOT(ISERROR(SEARCH("Non acquis",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="15" operator="containsText" text="En voie d'acquisition">
+    <cfRule type="containsText" dxfId="2" priority="25" operator="containsText" text="En voie d'acquisition">
       <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="16" operator="containsText" text="Acquis">
+    <cfRule type="containsText" dxfId="3" priority="26" operator="containsText" text="Acquis">
       <formula>NOT(ISERROR(SEARCH("Acquis",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1380,21 +2040,55 @@
     <cfRule type="expression" dxfId="0" priority="10">
       <formula>Classe!D3</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="20" operator="containsText" text="Non acquis">
+    <cfRule type="containsText" dxfId="1" priority="30" operator="containsText" text="Non acquis">
       <formula>NOT(ISERROR(SEARCH("Non acquis",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="21" operator="containsText" text="En voie d'acquisition">
+    <cfRule type="containsText" dxfId="2" priority="31" operator="containsText" text="En voie d'acquisition">
       <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="22" operator="containsText" text="Acquis">
+    <cfRule type="containsText" dxfId="3" priority="32" operator="containsText" text="Acquis">
       <formula>NOT(ISERROR(SEARCH("Acquis",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <conditionalFormatting sqref="E4">
+    <cfRule type="expression" dxfId="0" priority="15">
+      <formula>Classe!D4</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="36" operator="containsText" text="Non acquis">
+      <formula>NOT(ISERROR(SEARCH("Non acquis",E4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="37" operator="containsText" text="En voie d'acquisition">
+      <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",E4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="38" operator="containsText" text="Acquis">
+      <formula>NOT(ISERROR(SEARCH("Acquis",E4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="expression" dxfId="0" priority="20">
+      <formula>Classe!D5</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="42" operator="containsText" text="Non acquis">
+      <formula>NOT(ISERROR(SEARCH("Non acquis",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="43" operator="containsText" text="En voie d'acquisition">
+      <formula>NOT(ISERROR(SEARCH("En voie d'acquisition",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="44" operator="containsText" text="Acquis">
+      <formula>NOT(ISERROR(SEARCH("Acquis",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
       <formula1>"Non acquis,En voie d'acquisition,Acquis"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3">
+      <formula1>"Non acquis,En voie d'acquisition,Acquis"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">
+      <formula1>"Non acquis,En voie d'acquisition,Acquis"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5">
       <formula1>"Non acquis,En voie d'acquisition,Acquis"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>